<commit_message>
Tinh toan va do du lieu ve bao cao chi tiet
</commit_message>
<xml_diff>
--- a/Files/Tonghopquy.xlsx
+++ b/Files/Tonghopquy.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Viettel\Viettel_Report_Automation\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A2C018-6E1A-4D83-B609-9F86DF651E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038E791B-36FB-4CE7-BBEC-AAB1A001491B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC4FF3CA-F5B3-428F-9F7C-B436B672B428}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{DC4FF3CA-F5B3-428F-9F7C-B436B672B428}"/>
   </bookViews>
   <sheets>
     <sheet name="Quy I" sheetId="1" r:id="rId1"/>
     <sheet name="Quy II" sheetId="2" r:id="rId2"/>
     <sheet name="Quy III" sheetId="3" r:id="rId3"/>
     <sheet name="Quy IV" sheetId="4" r:id="rId4"/>
+    <sheet name="Nam" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
   <si>
     <t>Thang 1</t>
   </si>
@@ -76,13 +77,28 @@
   </si>
   <si>
     <t>Chỉ tiêu</t>
+  </si>
+  <si>
+    <t>Quý I</t>
+  </si>
+  <si>
+    <t>Quý II</t>
+  </si>
+  <si>
+    <t>Quý III</t>
+  </si>
+  <si>
+    <t>Quý IV</t>
+  </si>
+  <si>
+    <t>Tỏng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +106,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +123,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +203,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308C8235-9B6B-43CD-88BC-FB3810420C75}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H3" sqref="H3:I98"/>
     </sheetView>
   </sheetViews>
@@ -1084,4 +1118,85 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE663BA-9C07-43A5-A5F9-F068BBBD7BB6}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>